<commit_message>
Updated TC3 Results Rev E
</commit_message>
<xml_diff>
--- a/Test Case - 3/TC3_Results_E.xlsx
+++ b/Test Case - 3/TC3_Results_E.xlsx
@@ -1506,36 +1506,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1621,6 +1591,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2403,7 +2403,7 @@
   <dimension ref="A1:R112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,13 +3482,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="11">
-        <v>7.7</v>
+        <v>7.54</v>
       </c>
       <c r="C22" s="11">
-        <v>12.5</v>
+        <v>12.57</v>
       </c>
       <c r="D22" s="11">
-        <v>30</v>
+        <v>30.15</v>
       </c>
       <c r="E22" s="11">
         <v>7.5</v>
@@ -3506,14 +3506,14 @@
         <v>86</v>
       </c>
       <c r="J22" s="11">
-        <v>1</v>
+        <v>1.46</v>
       </c>
       <c r="K22" s="11">
         <v>1.48401472</v>
       </c>
       <c r="L22" s="11" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="11">
         <v>10.09</v>
@@ -3524,13 +3524,7 @@
       <c r="O22" s="11">
         <v>35.152000000000001</v>
       </c>
-      <c r="P22" s="2">
-        <f>0.9*((O22-D22)^0.51)*((SQRT((M22-B22)^2+(N22-C22)^2)^(-0.35)))</f>
-        <v>1.5304883323486536</v>
-      </c>
-      <c r="Q22" s="10" t="b">
-        <v>0</v>
-      </c>
+      <c r="Q22"/>
       <c r="R22" s="10" t="s">
         <v>18</v>
       </c>
@@ -3675,6 +3669,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="Q25" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="R25" s="10" t="s">
         <v>24</v>
       </c>
@@ -4235,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="10" t="s">
         <v>18</v>
@@ -4645,13 +4642,6 @@
       <c r="O44" s="11">
         <v>32.652000000000001</v>
       </c>
-      <c r="P44" s="2">
-        <f>0.9*((O44-D44)^0.51)*((SQRT((M44-B44)^2+(N44-C44)^2)^(-0.35)))</f>
-        <v>0.95002091522591725</v>
-      </c>
-      <c r="Q44" s="10" t="b">
-        <v>1</v>
-      </c>
       <c r="R44" s="10" t="s">
         <v>18</v>
       </c>
@@ -6768,6 +6758,13 @@
       </c>
       <c r="O84" s="11">
         <v>37.652000000000001</v>
+      </c>
+      <c r="P84" s="2">
+        <f>0.9*((O84-D84)^0.51)*((SQRT((M84-B84)^2+(N84-C84)^2)^(-0.35)))</f>
+        <v>1.0733170653684889</v>
+      </c>
+      <c r="Q84" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="R84" s="10" t="s">
         <v>53</v>
@@ -7973,47 +7970,47 @@
     <mergeCell ref="M1:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M24 R25 M26:M35 R36 M37:M90 R91:R110">
-    <cfRule type="cellIs" dxfId="70" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="95" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="96" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="97" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L112">
-    <cfRule type="cellIs" dxfId="67" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="81" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="82" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="77" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q44">
-    <cfRule type="cellIs" dxfId="62" priority="57" operator="equal">
+  <conditionalFormatting sqref="Q45">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="65" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q36">
+  <conditionalFormatting sqref="Q85">
     <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -8024,161 +8021,163 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q45">
-    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
+  <conditionalFormatting sqref="Q100">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="58" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="56" operator="greaterThan">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q85">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="53" operator="greaterThan">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q100">
-    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="59" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q47">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q50">
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="53" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q52">
-    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="50" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54">
-    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="47" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="44" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q60">
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q62">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q77">
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="35" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q78">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q82">
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="29" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q88">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q18">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q36">
     <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -8189,27 +8188,25 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+  <conditionalFormatting sqref="Q25">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+  <conditionalFormatting sqref="Q84">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8221,8 +8218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8772,10 +8769,15 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
+      <c r="T10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="V10" s="3" t="s">
         <v>130</v>
       </c>
@@ -9007,10 +9009,10 @@
         <v>5.2717991775013404</v>
       </c>
       <c r="K14" s="3">
-        <v>4.6143465762141398</v>
+        <v>5.3021987090120497</v>
       </c>
       <c r="L14" s="3">
-        <v>2.3659183666169099</v>
+        <v>2.71860145351204</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>130</v>
@@ -9033,7 +9035,7 @@
       </c>
       <c r="S14" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9149,10 +9151,10 @@
         <v>5.2717991775013404</v>
       </c>
       <c r="K16" s="3">
-        <v>4.6143465762141398</v>
+        <v>5.3021987090120497</v>
       </c>
       <c r="L16" s="3">
-        <v>2.3659183666169099</v>
+        <v>2.71860145351204</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>130</v>
@@ -9175,7 +9177,7 @@
       </c>
       <c r="S16" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9291,10 +9293,10 @@
         <v>5.2717991775013404</v>
       </c>
       <c r="K18" s="3">
-        <v>4.6143465762141398</v>
+        <v>5.3021987090120497</v>
       </c>
       <c r="L18" s="3">
-        <v>2.3659183666169099</v>
+        <v>2.71860145351204</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>130</v>
@@ -9317,7 +9319,7 @@
       </c>
       <c r="S18" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9362,10 +9364,10 @@
         <v>6.7568273967598698</v>
       </c>
       <c r="K19" s="3">
-        <v>4.0951600488032103</v>
+        <v>6.7741184759453796</v>
       </c>
       <c r="L19" s="3">
-        <v>2.3659183756864199</v>
+        <v>3.91364713230193</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>130</v>
@@ -9388,7 +9390,7 @@
       </c>
       <c r="S19" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9504,10 +9506,10 @@
         <v>6.7568273967598698</v>
       </c>
       <c r="K21" s="3">
-        <v>4.0951600488032103</v>
+        <v>6.7741184759453796</v>
       </c>
       <c r="L21" s="3">
-        <v>2.3659183756864199</v>
+        <v>3.91364713230193</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>130</v>
@@ -9530,7 +9532,7 @@
       </c>
       <c r="S21" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9646,10 +9648,10 @@
         <v>6.7568273967598698</v>
       </c>
       <c r="K23" s="3">
-        <v>4.0951600488032103</v>
+        <v>6.7741184759453796</v>
       </c>
       <c r="L23" s="3">
-        <v>2.3659183756864199</v>
+        <v>3.91364713230193</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>130</v>
@@ -9672,7 +9674,7 @@
       </c>
       <c r="S23" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="9" t="b">
         <f t="shared" si="3"/>
@@ -9805,8 +9807,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="9" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="3" t="s">
         <v>24</v>
@@ -10526,8 +10527,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="9" t="b">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="3" t="s">
         <v>18</v>
@@ -11153,10 +11153,10 @@
         <v>7.2611641048888602</v>
       </c>
       <c r="K46" s="3">
-        <v>4.1787243693587302</v>
+        <v>7.2784941780400896</v>
       </c>
       <c r="L46" s="3">
-        <v>2.4581624839479099</v>
+        <v>4.2816227505422004</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>130</v>
@@ -11179,7 +11179,7 @@
       </c>
       <c r="S46" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T46" s="9" t="b">
         <f t="shared" si="3"/>
@@ -11295,10 +11295,10 @@
         <v>7.2611641048888602</v>
       </c>
       <c r="K48" s="3">
-        <v>4.1787243693587302</v>
+        <v>7.2784941780400896</v>
       </c>
       <c r="L48" s="3">
-        <v>2.4581624839479099</v>
+        <v>4.2816227505422004</v>
       </c>
       <c r="M48" s="3" t="s">
         <v>130</v>
@@ -11321,7 +11321,7 @@
       </c>
       <c r="S48" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48" s="9" t="b">
         <f t="shared" si="3"/>
@@ -11437,10 +11437,10 @@
         <v>7.2611641048888602</v>
       </c>
       <c r="K50" s="3">
-        <v>4.1787243693587302</v>
+        <v>7.2784941780400896</v>
       </c>
       <c r="L50" s="3">
-        <v>2.4581624839479099</v>
+        <v>4.2816227505422004</v>
       </c>
       <c r="M50" s="3" t="s">
         <v>130</v>
@@ -11463,7 +11463,7 @@
       </c>
       <c r="S50" s="9" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="9" t="b">
         <f t="shared" si="3"/>
@@ -12873,10 +12873,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K72" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L72" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M72" s="3" t="s">
         <v>130</v>
@@ -12899,7 +12899,7 @@
       </c>
       <c r="S72" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T72" s="9" t="b">
         <f t="shared" si="6"/>
@@ -12944,10 +12944,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K73" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L73" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>130</v>
@@ -12970,7 +12970,7 @@
       </c>
       <c r="S73" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T73" s="9" t="b">
         <f t="shared" si="6"/>
@@ -13015,10 +13015,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K74" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L74" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>130</v>
@@ -13041,7 +13041,7 @@
       </c>
       <c r="S74" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T74" s="9" t="b">
         <f t="shared" si="6"/>
@@ -13086,10 +13086,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K75" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L75" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M75" s="3" t="s">
         <v>130</v>
@@ -13112,11 +13112,11 @@
       </c>
       <c r="S75" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T75" s="9" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U75" s="3" t="s">
         <v>53</v>
@@ -13352,10 +13352,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K79" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L79" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M79" s="3" t="s">
         <v>130</v>
@@ -13378,11 +13378,11 @@
       </c>
       <c r="S79" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T79" s="9" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U79" s="3" t="s">
         <v>53</v>
@@ -13423,10 +13423,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K80" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L80" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>130</v>
@@ -13449,7 +13449,7 @@
       </c>
       <c r="S80" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T80" s="9" t="b">
         <f t="shared" si="6"/>
@@ -13494,10 +13494,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K81" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L81" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M81" s="3" t="s">
         <v>130</v>
@@ -13520,7 +13520,7 @@
       </c>
       <c r="S81" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T81" s="9" t="b">
         <f t="shared" si="6"/>
@@ -13565,10 +13565,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K82" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L82" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M82" s="3" t="s">
         <v>130</v>
@@ -13591,7 +13591,7 @@
       </c>
       <c r="S82" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T82" s="9" t="b">
         <f t="shared" si="6"/>
@@ -13636,10 +13636,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K83" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L83" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M83" s="3" t="s">
         <v>130</v>
@@ -13662,11 +13662,11 @@
       </c>
       <c r="S83" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T83" s="9" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U83" s="3" t="s">
         <v>53</v>
@@ -13967,10 +13967,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K88" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L88" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M88" s="3" t="s">
         <v>130</v>
@@ -13993,7 +13993,7 @@
       </c>
       <c r="S88" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T88" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14038,10 +14038,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K89" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L89" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M89" s="3" t="s">
         <v>130</v>
@@ -14064,7 +14064,7 @@
       </c>
       <c r="S89" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T89" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14109,10 +14109,10 @@
         <v>7.5929160335216999</v>
       </c>
       <c r="K90" s="3">
-        <v>4.1842499858115696</v>
+        <v>7.60978102151575</v>
       </c>
       <c r="L90" s="3">
-        <v>2.5039841362289201</v>
+        <v>4.5539274715096898</v>
       </c>
       <c r="M90" s="3" t="s">
         <v>130</v>
@@ -14135,7 +14135,7 @@
       </c>
       <c r="S90" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T90" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14251,10 +14251,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K92" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L92" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M92" s="3" t="s">
         <v>130</v>
@@ -14277,7 +14277,7 @@
       </c>
       <c r="S92" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T92" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14322,10 +14322,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K93" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L93" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M93" s="3" t="s">
         <v>130</v>
@@ -14348,7 +14348,7 @@
       </c>
       <c r="S93" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T93" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14393,10 +14393,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K94" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L94" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M94" s="3" t="s">
         <v>130</v>
@@ -14419,7 +14419,7 @@
       </c>
       <c r="S94" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T94" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14535,10 +14535,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K96" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L96" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M96" s="3" t="s">
         <v>130</v>
@@ -14561,7 +14561,7 @@
       </c>
       <c r="S96" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T96" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14677,10 +14677,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K98" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L98" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M98" s="3" t="s">
         <v>130</v>
@@ -14703,7 +14703,7 @@
       </c>
       <c r="S98" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T98" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14748,10 +14748,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K99" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L99" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M99" s="3" t="s">
         <v>130</v>
@@ -14774,7 +14774,7 @@
       </c>
       <c r="S99" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T99" s="9" t="b">
         <f t="shared" si="6"/>
@@ -14848,8 +14848,7 @@
         <v>0</v>
       </c>
       <c r="T100" s="9" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U100" s="3" t="s">
         <v>94</v>
@@ -14961,10 +14960,10 @@
         <v>8.3516997011313592</v>
       </c>
       <c r="K102" s="3">
-        <v>4.3656152047128396</v>
+        <v>8.3692876601374699</v>
       </c>
       <c r="L102" s="3">
-        <v>2.6551469810672699</v>
+        <v>5.0901620556270002</v>
       </c>
       <c r="M102" s="3" t="s">
         <v>130</v>
@@ -14987,7 +14986,7 @@
       </c>
       <c r="S102" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T102" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15103,10 +15102,10 @@
         <v>8.3539121675145704</v>
       </c>
       <c r="K104" s="3">
-        <v>4.36651286088318</v>
+        <v>8.3715059279100306</v>
       </c>
       <c r="L104" s="3">
-        <v>2.6556929313993498</v>
+        <v>5.0915111958290904</v>
       </c>
       <c r="M104" s="3" t="s">
         <v>130</v>
@@ -15129,7 +15128,7 @@
       </c>
       <c r="S104" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T104" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15174,10 +15173,10 @@
         <v>8.3539121675145704</v>
       </c>
       <c r="K105" s="3">
-        <v>4.36651286088318</v>
+        <v>8.3715059279100306</v>
       </c>
       <c r="L105" s="3">
-        <v>2.6556929313993498</v>
+        <v>5.0915111958290904</v>
       </c>
       <c r="M105" s="3" t="s">
         <v>130</v>
@@ -15200,7 +15199,7 @@
       </c>
       <c r="S105" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T105" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15245,10 +15244,10 @@
         <v>8.3539121675145704</v>
       </c>
       <c r="K106" s="3">
-        <v>4.36651286088318</v>
+        <v>8.3715059279100306</v>
       </c>
       <c r="L106" s="3">
-        <v>2.6556929313993498</v>
+        <v>5.0915111958290904</v>
       </c>
       <c r="M106" s="3" t="s">
         <v>130</v>
@@ -15271,7 +15270,7 @@
       </c>
       <c r="S106" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T106" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15387,10 +15386,10 @@
         <v>8.3539121675145704</v>
       </c>
       <c r="K108" s="3">
-        <v>4.36651286088318</v>
+        <v>8.3715059279100306</v>
       </c>
       <c r="L108" s="3">
-        <v>2.6556929313993498</v>
+        <v>5.0915111958290904</v>
       </c>
       <c r="M108" s="3" t="s">
         <v>130</v>
@@ -15413,7 +15412,7 @@
       </c>
       <c r="S108" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T108" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15529,10 +15528,10 @@
         <v>8.3539121675145704</v>
       </c>
       <c r="K110" s="3">
-        <v>4.36651286088318</v>
+        <v>8.3715059279100306</v>
       </c>
       <c r="L110" s="3">
-        <v>2.6556929313993498</v>
+        <v>5.0915111958290904</v>
       </c>
       <c r="M110" s="3" t="s">
         <v>130</v>
@@ -15555,7 +15554,7 @@
       </c>
       <c r="S110" s="9" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T110" s="9" t="b">
         <f t="shared" si="6"/>
@@ -15618,7 +15617,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="O7" sqref="O7:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>